<commit_message>
last minor changes before sending to arno
</commit_message>
<xml_diff>
--- a/Backup calculation compPV.xlsx
+++ b/Backup calculation compPV.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieljansen/Desktop/paper/LCA_Paper/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="3860" windowWidth="22620" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Actuations when Even" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Embodied</t>
   </si>
@@ -75,6 +71,15 @@
   </si>
   <si>
     <t>calc for numb of actuations</t>
+  </si>
+  <si>
+    <t>Number of  Actuations</t>
+  </si>
+  <si>
+    <t>Find out when soft robotic actuators break even with servo motors</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -84,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,16 +112,57 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -124,19 +170,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -191,7 +285,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,7 +320,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -413,20 +507,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -449,7 +545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -475,7 +571,7 @@
         <v>2692</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -507,7 +603,7 @@
         <v>-9443.4755999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -540,7 +636,7 @@
         <v>225.87817680000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -571,7 +667,7 @@
         <v>235.61999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -597,7 +693,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -630,10 +726,10 @@
         <v>-6212.9774232</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -666,7 +762,7 @@
         <v>11600</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -699,7 +795,7 @@
         <v>-535.60150199999998</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -727,7 +823,7 @@
         <v>349.70300320000081</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -737,5 +833,230 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2675.4</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
+        <v>3251.2</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <f>-1021.8*20*0.4621</f>
+        <v>-9443.4755999999998</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <f>-1021.8*20*0.4621</f>
+        <v>-9443.4755999999998</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <f>0.31/1000*$B$18*54*365*20*0.4621</f>
+        <v>338.81726520000001</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <f>0.01/1000*$B$18*54*365*20*0.4621</f>
+        <v>10.929589200000001</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <f>(42.73+35.81)*3</f>
+        <v>235.61999999999998</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>77</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <f>SUM(B3:B7)</f>
+        <v>-6116.6383347999999</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <f>SUM(F3:F7)</f>
+        <v>-6094.8460107999999</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" ref="B10:H10" si="0">580*20</f>
+        <v>11600</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>11600</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f>B8/B10*1000</f>
+        <v>-527.29640817241375</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <f>F8/F10*1000</f>
+        <v>-525.41775955172409</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <f>0.31/1000*$B$18*54*365*20*0.4621</f>
+        <v>338.81726520000001</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="F16" s="1">
+        <f>F8-B8</f>
+        <v>21.792324000000008</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="6">
+        <f>F12-B12</f>
+        <v>1.8786486206896598</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all graphs ppt updated
</commit_message>
<xml_diff>
--- a/Backup calculation compPV.xlsx
+++ b/Backup calculation compPV.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="460" windowWidth="13340" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="13760" yWindow="460" windowWidth="13340" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,12 +87,6 @@
     <t>Pv-type</t>
   </si>
   <si>
-    <t>Static ASF ENTSO-E excl shading</t>
-  </si>
-  <si>
-    <t>Static ASF ENTSO-E incl shading</t>
-  </si>
-  <si>
     <t>Total Irradiation (kWh/m2/year)</t>
   </si>
   <si>
@@ -124,6 +118,12 @@
   </si>
   <si>
     <t>Total Power (kWh/year)</t>
+  </si>
+  <si>
+    <t>Orientated solar façade ENTSO-E excl shading</t>
+  </si>
+  <si>
+    <t>Orientated solar facade ASF ENTSO-E incl shading</t>
   </si>
 </sst>
 </file>
@@ -556,9 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -596,10 +594,10 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -830,31 +828,31 @@
         <v>9</v>
       </c>
       <c r="B9" s="11">
-        <f>518.1946*20</f>
+        <f t="shared" ref="B9:H9" si="2">518.1946*20</f>
         <v>10363.892</v>
       </c>
       <c r="C9" s="11">
-        <f>518.1946*20</f>
+        <f t="shared" si="2"/>
         <v>10363.892</v>
       </c>
       <c r="D9" s="11">
-        <f>518.1946*20</f>
+        <f t="shared" si="2"/>
         <v>10363.892</v>
       </c>
       <c r="E9" s="11">
-        <f>518.1946*20</f>
+        <f t="shared" si="2"/>
         <v>10363.892</v>
       </c>
       <c r="F9" s="11">
-        <f>518.1946*20</f>
+        <f t="shared" si="2"/>
         <v>10363.892</v>
       </c>
       <c r="G9" s="11">
-        <f>518.1946*20</f>
+        <f t="shared" si="2"/>
         <v>10363.892</v>
       </c>
       <c r="H9" s="11">
-        <f>518.1946*20</f>
+        <f t="shared" si="2"/>
         <v>10363.892</v>
       </c>
       <c r="I9" s="11">
@@ -875,15 +873,15 @@
         <v>-601.08474916566104</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" ref="C11:D11" si="2">C7/C9*1000</f>
+        <f t="shared" ref="C11:D11" si="3">C7/C9*1000</f>
         <v>310.10533270705639</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70.629121260622938</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" ref="E11" si="3">E7/E9*1000</f>
+        <f t="shared" ref="E11" si="4">E7/E9*1000</f>
         <v>-887.47736784597907</v>
       </c>
       <c r="F11" s="3">
@@ -912,18 +910,18 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>966</v>
@@ -937,7 +935,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>0.6944444444444442</v>
@@ -951,7 +949,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>0.38470000000000004</v>
@@ -965,7 +963,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>412.76374999999979</v>
@@ -979,7 +977,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>7.0000000000000007E-2</v>
@@ -993,7 +991,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" s="8">
         <v>0</v>
@@ -1008,7 +1006,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1022,7 +1020,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="10">
         <v>439.18062999999978</v>
@@ -1088,11 +1086,11 @@
         <v>4014.88</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" ref="C27:D27" si="4">SUM(C24:C26)</f>
+        <f t="shared" ref="C27:D27" si="5">SUM(C24:C26)</f>
         <v>2546.41</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1937.94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed graphs, edited text everywhere
</commit_message>
<xml_diff>
--- a/Backup calculation compPV.xlsx
+++ b/Backup calculation compPV.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieljansen/Desktop/paper/LCA_Paper/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="460" windowWidth="13340" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="640" windowWidth="27680" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Actuations when Even" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -546,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,11 +551,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
@@ -573,7 +568,7 @@
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -602,7 +597,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -634,7 +629,7 @@
         <v>2352.3000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -673,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -712,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -749,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -781,7 +776,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -822,10 +817,10 @@
         <v>2426.4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -866,7 +861,7 @@
         <v>9421.7200000000012</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -907,7 +902,7 @@
         <v>257.53259489774689</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -921,7 +916,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -935,7 +930,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -949,7 +944,7 @@
         <v>0.6944444444444442</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -963,7 +958,7 @@
         <v>0.38470000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -977,7 +972,7 @@
         <v>412.76374999999979</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -991,7 +986,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1006,7 +1001,7 @@
       </c>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1020,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
@@ -1034,10 +1029,10 @@
         <v>627.40089999999964</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1046,7 @@
         <v>1600.97</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1065,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1079,7 +1074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1093,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1107,7 +1102,7 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -1124,7 +1119,7 @@
         <v>1604.06</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
@@ -1144,6 +1139,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1155,7 +1155,7 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
@@ -1167,12 +1167,12 @@
     <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1196,7 +1196,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1214,7 +1214,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1232,7 +1232,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1283,10 +1283,10 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1304,7 +1304,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1358,5 +1358,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>